<commit_message>
[SPONGE] programming frame slider updates
</commit_message>
<xml_diff>
--- a/covid_dashboard/data/db_contacts.xlsx
+++ b/covid_dashboard/data/db_contacts.xlsx
@@ -15,7 +15,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="energy" localSheetId="0">Sheet1!$A$1:$AF$62</definedName>
+    <definedName name="energy" localSheetId="0">Sheet1!$A$1:$AF$63</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
@@ -70,7 +70,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1862" uniqueCount="363">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1892" uniqueCount="368">
   <si>
     <t>replica</t>
   </si>
@@ -1159,6 +1159,21 @@
   </si>
   <si>
     <t>200</t>
+  </si>
+  <si>
+    <t>MET77</t>
+  </si>
+  <si>
+    <t>MET</t>
+  </si>
+  <si>
+    <t>303</t>
+  </si>
+  <si>
+    <t>77</t>
+  </si>
+  <si>
+    <t>-5.6666</t>
   </si>
 </sst>
 </file>
@@ -1491,10 +1506,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AF62"/>
+  <dimension ref="A1:AF63"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D53" sqref="D53:D55"/>
+      <selection activeCell="V15" sqref="V15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2817,13 +2832,13 @@
         <v>14</v>
       </c>
       <c r="D14" s="4">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E14" s="3" t="s">
         <v>32</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>33</v>
+        <v>363</v>
       </c>
       <c r="G14" s="3" t="s">
         <v>34</v>
@@ -2835,7 +2850,7 @@
         <v>34</v>
       </c>
       <c r="J14" s="3" t="s">
-        <v>102</v>
+        <v>60</v>
       </c>
       <c r="K14" s="3" t="s">
         <v>34</v>
@@ -2844,7 +2859,7 @@
         <v>34</v>
       </c>
       <c r="M14" s="3" t="s">
-        <v>103</v>
+        <v>61</v>
       </c>
       <c r="N14" s="3" t="s">
         <v>34</v>
@@ -2853,7 +2868,7 @@
         <v>34</v>
       </c>
       <c r="P14" s="3" t="s">
-        <v>104</v>
+        <v>62</v>
       </c>
       <c r="Q14" s="3" t="s">
         <v>34</v>
@@ -2862,7 +2877,7 @@
         <v>34</v>
       </c>
       <c r="S14" s="3" t="s">
-        <v>105</v>
+        <v>63</v>
       </c>
       <c r="T14" s="3" t="s">
         <v>34</v>
@@ -2871,7 +2886,7 @@
         <v>34</v>
       </c>
       <c r="V14" s="3" t="s">
-        <v>106</v>
+        <v>367</v>
       </c>
       <c r="W14" s="3" t="s">
         <v>34</v>
@@ -2883,25 +2898,25 @@
         <v>40</v>
       </c>
       <c r="Z14" s="3" t="s">
-        <v>101</v>
+        <v>59</v>
       </c>
       <c r="AA14" s="3" t="s">
-        <v>359</v>
+        <v>42</v>
       </c>
       <c r="AB14" s="3" t="s">
-        <v>178</v>
+        <v>43</v>
       </c>
       <c r="AC14" s="3" t="s">
-        <v>360</v>
+        <v>44</v>
       </c>
       <c r="AD14" s="3" t="s">
-        <v>361</v>
+        <v>364</v>
       </c>
       <c r="AE14" s="3" t="s">
-        <v>199</v>
+        <v>365</v>
       </c>
       <c r="AF14" s="3" t="s">
-        <v>362</v>
+        <v>366</v>
       </c>
     </row>
     <row r="15" spans="1:32" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -2915,7 +2930,7 @@
         <v>14</v>
       </c>
       <c r="D15" s="4">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E15" s="3" t="s">
         <v>32</v>
@@ -2933,7 +2948,7 @@
         <v>34</v>
       </c>
       <c r="J15" s="3" t="s">
-        <v>251</v>
+        <v>102</v>
       </c>
       <c r="K15" s="3" t="s">
         <v>34</v>
@@ -2942,7 +2957,7 @@
         <v>34</v>
       </c>
       <c r="M15" s="3" t="s">
-        <v>252</v>
+        <v>103</v>
       </c>
       <c r="N15" s="3" t="s">
         <v>34</v>
@@ -2951,7 +2966,7 @@
         <v>34</v>
       </c>
       <c r="P15" s="3" t="s">
-        <v>253</v>
+        <v>104</v>
       </c>
       <c r="Q15" s="3" t="s">
         <v>34</v>
@@ -2960,7 +2975,7 @@
         <v>34</v>
       </c>
       <c r="S15" s="3" t="s">
-        <v>254</v>
+        <v>105</v>
       </c>
       <c r="T15" s="3" t="s">
         <v>34</v>
@@ -2969,7 +2984,7 @@
         <v>34</v>
       </c>
       <c r="V15" s="3" t="s">
-        <v>255</v>
+        <v>106</v>
       </c>
       <c r="W15" s="3" t="s">
         <v>34</v>
@@ -2981,7 +2996,7 @@
         <v>40</v>
       </c>
       <c r="Z15" s="3" t="s">
-        <v>41</v>
+        <v>101</v>
       </c>
       <c r="AA15" s="3" t="s">
         <v>359</v>
@@ -3013,7 +3028,7 @@
         <v>14</v>
       </c>
       <c r="D16" s="4">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E16" s="3" t="s">
         <v>32</v>
@@ -3031,7 +3046,7 @@
         <v>34</v>
       </c>
       <c r="J16" s="3" t="s">
-        <v>236</v>
+        <v>251</v>
       </c>
       <c r="K16" s="3" t="s">
         <v>34</v>
@@ -3040,7 +3055,7 @@
         <v>34</v>
       </c>
       <c r="M16" s="3" t="s">
-        <v>237</v>
+        <v>252</v>
       </c>
       <c r="N16" s="3" t="s">
         <v>34</v>
@@ -3049,7 +3064,7 @@
         <v>34</v>
       </c>
       <c r="P16" s="3" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="Q16" s="3" t="s">
         <v>34</v>
@@ -3058,7 +3073,7 @@
         <v>34</v>
       </c>
       <c r="S16" s="3" t="s">
-        <v>239</v>
+        <v>254</v>
       </c>
       <c r="T16" s="3" t="s">
         <v>34</v>
@@ -3067,7 +3082,7 @@
         <v>34</v>
       </c>
       <c r="V16" s="3" t="s">
-        <v>240</v>
+        <v>255</v>
       </c>
       <c r="W16" s="3" t="s">
         <v>34</v>
@@ -3079,7 +3094,7 @@
         <v>40</v>
       </c>
       <c r="Z16" s="3" t="s">
-        <v>74</v>
+        <v>41</v>
       </c>
       <c r="AA16" s="3" t="s">
         <v>359</v>
@@ -3111,7 +3126,7 @@
         <v>14</v>
       </c>
       <c r="D17" s="4">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E17" s="3" t="s">
         <v>32</v>
@@ -3129,7 +3144,7 @@
         <v>34</v>
       </c>
       <c r="J17" s="3" t="s">
-        <v>128</v>
+        <v>236</v>
       </c>
       <c r="K17" s="3" t="s">
         <v>34</v>
@@ -3138,7 +3153,7 @@
         <v>34</v>
       </c>
       <c r="M17" s="3" t="s">
-        <v>129</v>
+        <v>237</v>
       </c>
       <c r="N17" s="3" t="s">
         <v>34</v>
@@ -3147,7 +3162,7 @@
         <v>34</v>
       </c>
       <c r="P17" s="3" t="s">
-        <v>130</v>
+        <v>238</v>
       </c>
       <c r="Q17" s="3" t="s">
         <v>34</v>
@@ -3156,7 +3171,7 @@
         <v>34</v>
       </c>
       <c r="S17" s="3" t="s">
-        <v>131</v>
+        <v>239</v>
       </c>
       <c r="T17" s="3" t="s">
         <v>34</v>
@@ -3165,7 +3180,7 @@
         <v>34</v>
       </c>
       <c r="V17" s="3" t="s">
-        <v>132</v>
+        <v>240</v>
       </c>
       <c r="W17" s="3" t="s">
         <v>34</v>
@@ -3180,119 +3195,119 @@
         <v>74</v>
       </c>
       <c r="AA17" s="3" t="s">
+        <v>359</v>
+      </c>
+      <c r="AB17" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="AC17" s="3" t="s">
+        <v>360</v>
+      </c>
+      <c r="AD17" s="3" t="s">
+        <v>361</v>
+      </c>
+      <c r="AE17" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="AF17" s="3" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="18" spans="1:32" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
+        <v>358</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C18" s="4">
+        <v>14</v>
+      </c>
+      <c r="D18" s="4">
+        <v>15</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="G18" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="H18" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="I18" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="J18" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="K18" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="L18" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="M18" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="N18" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="O18" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="P18" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="Q18" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="R18" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="S18" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="T18" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="U18" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="V18" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="W18" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="X18" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="Y18" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="Z18" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="AA18" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="AB17" s="3" t="s">
+      <c r="AB18" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="AC17" s="3" t="s">
+      <c r="AC18" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="AD17" s="3" t="s">
+      <c r="AD18" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="AE17" s="3" t="s">
+      <c r="AE18" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="AF17" s="3" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="18" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
-        <v>358</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C18" s="2">
-        <v>14</v>
-      </c>
-      <c r="D18" s="2">
-        <v>16</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="F18" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="G18" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="H18" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="I18" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="J18" s="1" t="s">
-        <v>221</v>
-      </c>
-      <c r="K18" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="L18" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="M18" s="1" t="s">
-        <v>222</v>
-      </c>
-      <c r="N18" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="O18" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="P18" s="1" t="s">
-        <v>223</v>
-      </c>
-      <c r="Q18" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="R18" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="S18" s="1" t="s">
-        <v>224</v>
-      </c>
-      <c r="T18" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="U18" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="V18" s="1" t="s">
-        <v>225</v>
-      </c>
-      <c r="W18" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="X18" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="Y18" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="Z18" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="AA18" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="AB18" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="AC18" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="AD18" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="AE18" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="AF18" s="1" t="s">
+      <c r="AF18" s="3" t="s">
         <v>47</v>
       </c>
     </row>
@@ -3307,7 +3322,7 @@
         <v>14</v>
       </c>
       <c r="D19" s="2">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E19" s="1" t="s">
         <v>32</v>
@@ -3325,7 +3340,7 @@
         <v>34</v>
       </c>
       <c r="J19" s="1" t="s">
-        <v>210</v>
+        <v>221</v>
       </c>
       <c r="K19" s="1" t="s">
         <v>34</v>
@@ -3334,7 +3349,7 @@
         <v>34</v>
       </c>
       <c r="M19" s="1" t="s">
-        <v>211</v>
+        <v>222</v>
       </c>
       <c r="N19" s="1" t="s">
         <v>34</v>
@@ -3343,7 +3358,7 @@
         <v>34</v>
       </c>
       <c r="P19" s="1" t="s">
-        <v>212</v>
+        <v>223</v>
       </c>
       <c r="Q19" s="1" t="s">
         <v>34</v>
@@ -3352,7 +3367,7 @@
         <v>34</v>
       </c>
       <c r="S19" s="1" t="s">
-        <v>213</v>
+        <v>224</v>
       </c>
       <c r="T19" s="1" t="s">
         <v>34</v>
@@ -3361,7 +3376,7 @@
         <v>34</v>
       </c>
       <c r="V19" s="1" t="s">
-        <v>214</v>
+        <v>225</v>
       </c>
       <c r="W19" s="1" t="s">
         <v>34</v>
@@ -3373,7 +3388,7 @@
         <v>40</v>
       </c>
       <c r="Z19" s="1" t="s">
-        <v>157</v>
+        <v>41</v>
       </c>
       <c r="AA19" s="1" t="s">
         <v>42</v>
@@ -3405,7 +3420,7 @@
         <v>14</v>
       </c>
       <c r="D20" s="2">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E20" s="1" t="s">
         <v>32</v>
@@ -3423,7 +3438,7 @@
         <v>34</v>
       </c>
       <c r="J20" s="1" t="s">
-        <v>286</v>
+        <v>210</v>
       </c>
       <c r="K20" s="1" t="s">
         <v>34</v>
@@ -3432,7 +3447,7 @@
         <v>34</v>
       </c>
       <c r="M20" s="1" t="s">
-        <v>287</v>
+        <v>211</v>
       </c>
       <c r="N20" s="1" t="s">
         <v>34</v>
@@ -3441,7 +3456,7 @@
         <v>34</v>
       </c>
       <c r="P20" s="1" t="s">
-        <v>288</v>
+        <v>212</v>
       </c>
       <c r="Q20" s="1" t="s">
         <v>34</v>
@@ -3450,7 +3465,7 @@
         <v>34</v>
       </c>
       <c r="S20" s="1" t="s">
-        <v>289</v>
+        <v>213</v>
       </c>
       <c r="T20" s="1" t="s">
         <v>34</v>
@@ -3459,7 +3474,7 @@
         <v>34</v>
       </c>
       <c r="V20" s="1" t="s">
-        <v>290</v>
+        <v>214</v>
       </c>
       <c r="W20" s="1" t="s">
         <v>34</v>
@@ -3471,7 +3486,7 @@
         <v>40</v>
       </c>
       <c r="Z20" s="1" t="s">
-        <v>59</v>
+        <v>157</v>
       </c>
       <c r="AA20" s="1" t="s">
         <v>42</v>
@@ -3503,7 +3518,7 @@
         <v>14</v>
       </c>
       <c r="D21" s="2">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E21" s="1" t="s">
         <v>32</v>
@@ -3521,7 +3536,7 @@
         <v>34</v>
       </c>
       <c r="J21" s="1" t="s">
-        <v>123</v>
+        <v>286</v>
       </c>
       <c r="K21" s="1" t="s">
         <v>34</v>
@@ -3530,7 +3545,7 @@
         <v>34</v>
       </c>
       <c r="M21" s="1" t="s">
-        <v>124</v>
+        <v>287</v>
       </c>
       <c r="N21" s="1" t="s">
         <v>34</v>
@@ -3539,7 +3554,7 @@
         <v>34</v>
       </c>
       <c r="P21" s="1" t="s">
-        <v>125</v>
+        <v>288</v>
       </c>
       <c r="Q21" s="1" t="s">
         <v>34</v>
@@ -3548,7 +3563,7 @@
         <v>34</v>
       </c>
       <c r="S21" s="1" t="s">
-        <v>126</v>
+        <v>289</v>
       </c>
       <c r="T21" s="1" t="s">
         <v>34</v>
@@ -3557,7 +3572,7 @@
         <v>34</v>
       </c>
       <c r="V21" s="1" t="s">
-        <v>127</v>
+        <v>290</v>
       </c>
       <c r="W21" s="1" t="s">
         <v>34</v>
@@ -3569,7 +3584,7 @@
         <v>40</v>
       </c>
       <c r="Z21" s="1" t="s">
-        <v>85</v>
+        <v>59</v>
       </c>
       <c r="AA21" s="1" t="s">
         <v>42</v>
@@ -3601,7 +3616,7 @@
         <v>14</v>
       </c>
       <c r="D22" s="2">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E22" s="1" t="s">
         <v>32</v>
@@ -3619,7 +3634,7 @@
         <v>34</v>
       </c>
       <c r="J22" s="1" t="s">
-        <v>143</v>
+        <v>123</v>
       </c>
       <c r="K22" s="1" t="s">
         <v>34</v>
@@ -3628,7 +3643,7 @@
         <v>34</v>
       </c>
       <c r="M22" s="1" t="s">
-        <v>144</v>
+        <v>124</v>
       </c>
       <c r="N22" s="1" t="s">
         <v>34</v>
@@ -3637,7 +3652,7 @@
         <v>34</v>
       </c>
       <c r="P22" s="1" t="s">
-        <v>145</v>
+        <v>125</v>
       </c>
       <c r="Q22" s="1" t="s">
         <v>34</v>
@@ -3646,7 +3661,7 @@
         <v>34</v>
       </c>
       <c r="S22" s="1" t="s">
-        <v>146</v>
+        <v>126</v>
       </c>
       <c r="T22" s="1" t="s">
         <v>34</v>
@@ -3655,7 +3670,7 @@
         <v>34</v>
       </c>
       <c r="V22" s="1" t="s">
-        <v>147</v>
+        <v>127</v>
       </c>
       <c r="W22" s="1" t="s">
         <v>34</v>
@@ -3667,7 +3682,7 @@
         <v>40</v>
       </c>
       <c r="Z22" s="1" t="s">
-        <v>53</v>
+        <v>85</v>
       </c>
       <c r="AA22" s="1" t="s">
         <v>42</v>
@@ -3699,7 +3714,7 @@
         <v>14</v>
       </c>
       <c r="D23" s="2">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E23" s="1" t="s">
         <v>32</v>
@@ -3717,7 +3732,7 @@
         <v>34</v>
       </c>
       <c r="J23" s="1" t="s">
-        <v>194</v>
+        <v>143</v>
       </c>
       <c r="K23" s="1" t="s">
         <v>34</v>
@@ -3726,7 +3741,7 @@
         <v>34</v>
       </c>
       <c r="M23" s="1" t="s">
-        <v>195</v>
+        <v>144</v>
       </c>
       <c r="N23" s="1" t="s">
         <v>34</v>
@@ -3735,7 +3750,7 @@
         <v>34</v>
       </c>
       <c r="P23" s="1" t="s">
-        <v>196</v>
+        <v>145</v>
       </c>
       <c r="Q23" s="1" t="s">
         <v>34</v>
@@ -3744,7 +3759,7 @@
         <v>34</v>
       </c>
       <c r="S23" s="1" t="s">
-        <v>197</v>
+        <v>146</v>
       </c>
       <c r="T23" s="1" t="s">
         <v>34</v>
@@ -3753,7 +3768,7 @@
         <v>34</v>
       </c>
       <c r="V23" s="1" t="s">
-        <v>198</v>
+        <v>147</v>
       </c>
       <c r="W23" s="1" t="s">
         <v>34</v>
@@ -3765,7 +3780,7 @@
         <v>40</v>
       </c>
       <c r="Z23" s="1" t="s">
-        <v>85</v>
+        <v>53</v>
       </c>
       <c r="AA23" s="1" t="s">
         <v>42</v>
@@ -3797,7 +3812,7 @@
         <v>14</v>
       </c>
       <c r="D24" s="2">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E24" s="1" t="s">
         <v>32</v>
@@ -3815,7 +3830,7 @@
         <v>34</v>
       </c>
       <c r="J24" s="1" t="s">
-        <v>302</v>
+        <v>194</v>
       </c>
       <c r="K24" s="1" t="s">
         <v>34</v>
@@ -3824,7 +3839,7 @@
         <v>34</v>
       </c>
       <c r="M24" s="1" t="s">
-        <v>303</v>
+        <v>195</v>
       </c>
       <c r="N24" s="1" t="s">
         <v>34</v>
@@ -3833,7 +3848,7 @@
         <v>34</v>
       </c>
       <c r="P24" s="1" t="s">
-        <v>304</v>
+        <v>196</v>
       </c>
       <c r="Q24" s="1" t="s">
         <v>34</v>
@@ -3842,7 +3857,7 @@
         <v>34</v>
       </c>
       <c r="S24" s="1" t="s">
-        <v>305</v>
+        <v>197</v>
       </c>
       <c r="T24" s="1" t="s">
         <v>34</v>
@@ -3851,7 +3866,7 @@
         <v>34</v>
       </c>
       <c r="V24" s="1" t="s">
-        <v>306</v>
+        <v>198</v>
       </c>
       <c r="W24" s="1" t="s">
         <v>34</v>
@@ -3895,7 +3910,7 @@
         <v>14</v>
       </c>
       <c r="D25" s="2">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E25" s="1" t="s">
         <v>32</v>
@@ -3913,7 +3928,7 @@
         <v>34</v>
       </c>
       <c r="J25" s="1" t="s">
-        <v>189</v>
+        <v>302</v>
       </c>
       <c r="K25" s="1" t="s">
         <v>34</v>
@@ -3922,7 +3937,7 @@
         <v>34</v>
       </c>
       <c r="M25" s="1" t="s">
-        <v>190</v>
+        <v>303</v>
       </c>
       <c r="N25" s="1" t="s">
         <v>34</v>
@@ -3931,7 +3946,7 @@
         <v>34</v>
       </c>
       <c r="P25" s="1" t="s">
-        <v>191</v>
+        <v>304</v>
       </c>
       <c r="Q25" s="1" t="s">
         <v>34</v>
@@ -3940,7 +3955,7 @@
         <v>34</v>
       </c>
       <c r="S25" s="1" t="s">
-        <v>192</v>
+        <v>305</v>
       </c>
       <c r="T25" s="1" t="s">
         <v>34</v>
@@ -3949,7 +3964,7 @@
         <v>34</v>
       </c>
       <c r="V25" s="1" t="s">
-        <v>193</v>
+        <v>306</v>
       </c>
       <c r="W25" s="1" t="s">
         <v>34</v>
@@ -3961,7 +3976,7 @@
         <v>40</v>
       </c>
       <c r="Z25" s="1" t="s">
-        <v>59</v>
+        <v>85</v>
       </c>
       <c r="AA25" s="1" t="s">
         <v>42</v>
@@ -3993,7 +4008,7 @@
         <v>14</v>
       </c>
       <c r="D26" s="2">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E26" s="1" t="s">
         <v>32</v>
@@ -4011,7 +4026,7 @@
         <v>34</v>
       </c>
       <c r="J26" s="1" t="s">
-        <v>152</v>
+        <v>189</v>
       </c>
       <c r="K26" s="1" t="s">
         <v>34</v>
@@ -4020,7 +4035,7 @@
         <v>34</v>
       </c>
       <c r="M26" s="1" t="s">
-        <v>153</v>
+        <v>190</v>
       </c>
       <c r="N26" s="1" t="s">
         <v>34</v>
@@ -4029,7 +4044,7 @@
         <v>34</v>
       </c>
       <c r="P26" s="1" t="s">
-        <v>154</v>
+        <v>191</v>
       </c>
       <c r="Q26" s="1" t="s">
         <v>34</v>
@@ -4038,7 +4053,7 @@
         <v>34</v>
       </c>
       <c r="S26" s="1" t="s">
-        <v>155</v>
+        <v>192</v>
       </c>
       <c r="T26" s="1" t="s">
         <v>34</v>
@@ -4047,7 +4062,7 @@
         <v>34</v>
       </c>
       <c r="V26" s="1" t="s">
-        <v>156</v>
+        <v>193</v>
       </c>
       <c r="W26" s="1" t="s">
         <v>34</v>
@@ -4059,7 +4074,7 @@
         <v>40</v>
       </c>
       <c r="Z26" s="1" t="s">
-        <v>157</v>
+        <v>59</v>
       </c>
       <c r="AA26" s="1" t="s">
         <v>42</v>
@@ -4091,7 +4106,7 @@
         <v>14</v>
       </c>
       <c r="D27" s="2">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E27" s="1" t="s">
         <v>32</v>
@@ -4109,7 +4124,7 @@
         <v>34</v>
       </c>
       <c r="J27" s="1" t="s">
-        <v>200</v>
+        <v>152</v>
       </c>
       <c r="K27" s="1" t="s">
         <v>34</v>
@@ -4118,7 +4133,7 @@
         <v>34</v>
       </c>
       <c r="M27" s="1" t="s">
-        <v>201</v>
+        <v>153</v>
       </c>
       <c r="N27" s="1" t="s">
         <v>34</v>
@@ -4127,7 +4142,7 @@
         <v>34</v>
       </c>
       <c r="P27" s="1" t="s">
-        <v>202</v>
+        <v>154</v>
       </c>
       <c r="Q27" s="1" t="s">
         <v>34</v>
@@ -4136,7 +4151,7 @@
         <v>34</v>
       </c>
       <c r="S27" s="1" t="s">
-        <v>203</v>
+        <v>155</v>
       </c>
       <c r="T27" s="1" t="s">
         <v>34</v>
@@ -4145,7 +4160,7 @@
         <v>34</v>
       </c>
       <c r="V27" s="1" t="s">
-        <v>204</v>
+        <v>156</v>
       </c>
       <c r="W27" s="1" t="s">
         <v>34</v>
@@ -4157,7 +4172,7 @@
         <v>40</v>
       </c>
       <c r="Z27" s="1" t="s">
-        <v>74</v>
+        <v>157</v>
       </c>
       <c r="AA27" s="1" t="s">
         <v>42</v>
@@ -4189,7 +4204,7 @@
         <v>14</v>
       </c>
       <c r="D28" s="2">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E28" s="1" t="s">
         <v>32</v>
@@ -4207,7 +4222,7 @@
         <v>34</v>
       </c>
       <c r="J28" s="1" t="s">
-        <v>35</v>
+        <v>200</v>
       </c>
       <c r="K28" s="1" t="s">
         <v>34</v>
@@ -4216,7 +4231,7 @@
         <v>34</v>
       </c>
       <c r="M28" s="1" t="s">
-        <v>36</v>
+        <v>201</v>
       </c>
       <c r="N28" s="1" t="s">
         <v>34</v>
@@ -4225,7 +4240,7 @@
         <v>34</v>
       </c>
       <c r="P28" s="1" t="s">
-        <v>37</v>
+        <v>202</v>
       </c>
       <c r="Q28" s="1" t="s">
         <v>34</v>
@@ -4234,7 +4249,7 @@
         <v>34</v>
       </c>
       <c r="S28" s="1" t="s">
-        <v>38</v>
+        <v>203</v>
       </c>
       <c r="T28" s="1" t="s">
         <v>34</v>
@@ -4243,7 +4258,7 @@
         <v>34</v>
       </c>
       <c r="V28" s="1" t="s">
-        <v>39</v>
+        <v>204</v>
       </c>
       <c r="W28" s="1" t="s">
         <v>34</v>
@@ -4255,7 +4270,7 @@
         <v>40</v>
       </c>
       <c r="Z28" s="1" t="s">
-        <v>41</v>
+        <v>74</v>
       </c>
       <c r="AA28" s="1" t="s">
         <v>42</v>
@@ -4287,7 +4302,7 @@
         <v>14</v>
       </c>
       <c r="D29" s="2">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E29" s="1" t="s">
         <v>32</v>
@@ -4305,7 +4320,7 @@
         <v>34</v>
       </c>
       <c r="J29" s="1" t="s">
-        <v>107</v>
+        <v>35</v>
       </c>
       <c r="K29" s="1" t="s">
         <v>34</v>
@@ -4314,7 +4329,7 @@
         <v>34</v>
       </c>
       <c r="M29" s="1" t="s">
-        <v>108</v>
+        <v>36</v>
       </c>
       <c r="N29" s="1" t="s">
         <v>34</v>
@@ -4323,7 +4338,7 @@
         <v>34</v>
       </c>
       <c r="P29" s="1" t="s">
-        <v>109</v>
+        <v>37</v>
       </c>
       <c r="Q29" s="1" t="s">
         <v>34</v>
@@ -4332,7 +4347,7 @@
         <v>34</v>
       </c>
       <c r="S29" s="1" t="s">
-        <v>110</v>
+        <v>38</v>
       </c>
       <c r="T29" s="1" t="s">
         <v>34</v>
@@ -4341,7 +4356,7 @@
         <v>34</v>
       </c>
       <c r="V29" s="1" t="s">
-        <v>111</v>
+        <v>39</v>
       </c>
       <c r="W29" s="1" t="s">
         <v>34</v>
@@ -4353,7 +4368,7 @@
         <v>40</v>
       </c>
       <c r="Z29" s="1" t="s">
-        <v>101</v>
+        <v>41</v>
       </c>
       <c r="AA29" s="1" t="s">
         <v>42</v>
@@ -4385,7 +4400,7 @@
         <v>14</v>
       </c>
       <c r="D30" s="2">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E30" s="1" t="s">
         <v>32</v>
@@ -4403,7 +4418,7 @@
         <v>34</v>
       </c>
       <c r="J30" s="1" t="s">
-        <v>215</v>
+        <v>107</v>
       </c>
       <c r="K30" s="1" t="s">
         <v>34</v>
@@ -4412,7 +4427,7 @@
         <v>34</v>
       </c>
       <c r="M30" s="1" t="s">
-        <v>216</v>
+        <v>108</v>
       </c>
       <c r="N30" s="1" t="s">
         <v>34</v>
@@ -4421,7 +4436,7 @@
         <v>34</v>
       </c>
       <c r="P30" s="1" t="s">
-        <v>217</v>
+        <v>109</v>
       </c>
       <c r="Q30" s="1" t="s">
         <v>34</v>
@@ -4430,7 +4445,7 @@
         <v>34</v>
       </c>
       <c r="S30" s="1" t="s">
-        <v>218</v>
+        <v>110</v>
       </c>
       <c r="T30" s="1" t="s">
         <v>34</v>
@@ -4439,7 +4454,7 @@
         <v>34</v>
       </c>
       <c r="V30" s="1" t="s">
-        <v>219</v>
+        <v>111</v>
       </c>
       <c r="W30" s="1" t="s">
         <v>34</v>
@@ -4451,7 +4466,7 @@
         <v>40</v>
       </c>
       <c r="Z30" s="1" t="s">
-        <v>220</v>
+        <v>101</v>
       </c>
       <c r="AA30" s="1" t="s">
         <v>42</v>
@@ -4483,7 +4498,7 @@
         <v>14</v>
       </c>
       <c r="D31" s="2">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E31" s="1" t="s">
         <v>32</v>
@@ -4501,7 +4516,7 @@
         <v>34</v>
       </c>
       <c r="J31" s="1" t="s">
-        <v>241</v>
+        <v>215</v>
       </c>
       <c r="K31" s="1" t="s">
         <v>34</v>
@@ -4510,7 +4525,7 @@
         <v>34</v>
       </c>
       <c r="M31" s="1" t="s">
-        <v>242</v>
+        <v>216</v>
       </c>
       <c r="N31" s="1" t="s">
         <v>34</v>
@@ -4519,7 +4534,7 @@
         <v>34</v>
       </c>
       <c r="P31" s="1" t="s">
-        <v>243</v>
+        <v>217</v>
       </c>
       <c r="Q31" s="1" t="s">
         <v>34</v>
@@ -4528,7 +4543,7 @@
         <v>34</v>
       </c>
       <c r="S31" s="1" t="s">
-        <v>244</v>
+        <v>218</v>
       </c>
       <c r="T31" s="1" t="s">
         <v>34</v>
@@ -4537,7 +4552,7 @@
         <v>34</v>
       </c>
       <c r="V31" s="1" t="s">
-        <v>245</v>
+        <v>219</v>
       </c>
       <c r="W31" s="1" t="s">
         <v>34</v>
@@ -4549,7 +4564,7 @@
         <v>40</v>
       </c>
       <c r="Z31" s="1" t="s">
-        <v>74</v>
+        <v>220</v>
       </c>
       <c r="AA31" s="1" t="s">
         <v>42</v>
@@ -4581,7 +4596,7 @@
         <v>14</v>
       </c>
       <c r="D32" s="2">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E32" s="1" t="s">
         <v>32</v>
@@ -4599,7 +4614,7 @@
         <v>34</v>
       </c>
       <c r="J32" s="1" t="s">
-        <v>75</v>
+        <v>241</v>
       </c>
       <c r="K32" s="1" t="s">
         <v>34</v>
@@ -4608,7 +4623,7 @@
         <v>34</v>
       </c>
       <c r="M32" s="1" t="s">
-        <v>76</v>
+        <v>242</v>
       </c>
       <c r="N32" s="1" t="s">
         <v>34</v>
@@ -4617,7 +4632,7 @@
         <v>34</v>
       </c>
       <c r="P32" s="1" t="s">
-        <v>77</v>
+        <v>243</v>
       </c>
       <c r="Q32" s="1" t="s">
         <v>34</v>
@@ -4626,7 +4641,7 @@
         <v>34</v>
       </c>
       <c r="S32" s="1" t="s">
-        <v>78</v>
+        <v>244</v>
       </c>
       <c r="T32" s="1" t="s">
         <v>34</v>
@@ -4635,7 +4650,7 @@
         <v>34</v>
       </c>
       <c r="V32" s="1" t="s">
-        <v>79</v>
+        <v>245</v>
       </c>
       <c r="W32" s="1" t="s">
         <v>34</v>
@@ -4647,7 +4662,7 @@
         <v>40</v>
       </c>
       <c r="Z32" s="1" t="s">
-        <v>59</v>
+        <v>74</v>
       </c>
       <c r="AA32" s="1" t="s">
         <v>42</v>
@@ -4679,7 +4694,7 @@
         <v>14</v>
       </c>
       <c r="D33" s="2">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E33" s="1" t="s">
         <v>32</v>
@@ -4697,7 +4712,7 @@
         <v>34</v>
       </c>
       <c r="J33" s="1" t="s">
-        <v>231</v>
+        <v>75</v>
       </c>
       <c r="K33" s="1" t="s">
         <v>34</v>
@@ -4706,7 +4721,7 @@
         <v>34</v>
       </c>
       <c r="M33" s="1" t="s">
-        <v>232</v>
+        <v>76</v>
       </c>
       <c r="N33" s="1" t="s">
         <v>34</v>
@@ -4715,7 +4730,7 @@
         <v>34</v>
       </c>
       <c r="P33" s="1" t="s">
-        <v>233</v>
+        <v>77</v>
       </c>
       <c r="Q33" s="1" t="s">
         <v>34</v>
@@ -4724,7 +4739,7 @@
         <v>34</v>
       </c>
       <c r="S33" s="1" t="s">
-        <v>234</v>
+        <v>78</v>
       </c>
       <c r="T33" s="1" t="s">
         <v>34</v>
@@ -4733,7 +4748,7 @@
         <v>34</v>
       </c>
       <c r="V33" s="1" t="s">
-        <v>235</v>
+        <v>79</v>
       </c>
       <c r="W33" s="1" t="s">
         <v>34</v>
@@ -4745,7 +4760,7 @@
         <v>40</v>
       </c>
       <c r="Z33" s="1" t="s">
-        <v>157</v>
+        <v>59</v>
       </c>
       <c r="AA33" s="1" t="s">
         <v>42</v>
@@ -4777,7 +4792,7 @@
         <v>14</v>
       </c>
       <c r="D34" s="2">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E34" s="1" t="s">
         <v>32</v>
@@ -4795,7 +4810,7 @@
         <v>34</v>
       </c>
       <c r="J34" s="1" t="s">
-        <v>205</v>
+        <v>231</v>
       </c>
       <c r="K34" s="1" t="s">
         <v>34</v>
@@ -4804,7 +4819,7 @@
         <v>34</v>
       </c>
       <c r="M34" s="1" t="s">
-        <v>206</v>
+        <v>232</v>
       </c>
       <c r="N34" s="1" t="s">
         <v>34</v>
@@ -4813,7 +4828,7 @@
         <v>34</v>
       </c>
       <c r="P34" s="1" t="s">
-        <v>207</v>
+        <v>233</v>
       </c>
       <c r="Q34" s="1" t="s">
         <v>34</v>
@@ -4822,7 +4837,7 @@
         <v>34</v>
       </c>
       <c r="S34" s="1" t="s">
-        <v>208</v>
+        <v>234</v>
       </c>
       <c r="T34" s="1" t="s">
         <v>34</v>
@@ -4831,7 +4846,7 @@
         <v>34</v>
       </c>
       <c r="V34" s="1" t="s">
-        <v>209</v>
+        <v>235</v>
       </c>
       <c r="W34" s="1" t="s">
         <v>34</v>
@@ -4875,7 +4890,7 @@
         <v>14</v>
       </c>
       <c r="D35" s="2">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E35" s="1" t="s">
         <v>32</v>
@@ -4893,7 +4908,7 @@
         <v>34</v>
       </c>
       <c r="J35" s="1" t="s">
-        <v>91</v>
+        <v>205</v>
       </c>
       <c r="K35" s="1" t="s">
         <v>34</v>
@@ -4902,7 +4917,7 @@
         <v>34</v>
       </c>
       <c r="M35" s="1" t="s">
-        <v>92</v>
+        <v>206</v>
       </c>
       <c r="N35" s="1" t="s">
         <v>34</v>
@@ -4911,7 +4926,7 @@
         <v>34</v>
       </c>
       <c r="P35" s="1" t="s">
-        <v>93</v>
+        <v>207</v>
       </c>
       <c r="Q35" s="1" t="s">
         <v>34</v>
@@ -4920,7 +4935,7 @@
         <v>34</v>
       </c>
       <c r="S35" s="1" t="s">
-        <v>94</v>
+        <v>208</v>
       </c>
       <c r="T35" s="1" t="s">
         <v>34</v>
@@ -4929,7 +4944,7 @@
         <v>34</v>
       </c>
       <c r="V35" s="1" t="s">
-        <v>95</v>
+        <v>209</v>
       </c>
       <c r="W35" s="1" t="s">
         <v>34</v>
@@ -4941,7 +4956,7 @@
         <v>40</v>
       </c>
       <c r="Z35" s="1" t="s">
-        <v>41</v>
+        <v>157</v>
       </c>
       <c r="AA35" s="1" t="s">
         <v>42</v>
@@ -4973,7 +4988,7 @@
         <v>14</v>
       </c>
       <c r="D36" s="2">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E36" s="1" t="s">
         <v>32</v>
@@ -4991,7 +5006,7 @@
         <v>34</v>
       </c>
       <c r="J36" s="1" t="s">
-        <v>246</v>
+        <v>91</v>
       </c>
       <c r="K36" s="1" t="s">
         <v>34</v>
@@ -5000,7 +5015,7 @@
         <v>34</v>
       </c>
       <c r="M36" s="1" t="s">
-        <v>247</v>
+        <v>92</v>
       </c>
       <c r="N36" s="1" t="s">
         <v>34</v>
@@ -5009,7 +5024,7 @@
         <v>34</v>
       </c>
       <c r="P36" s="1" t="s">
-        <v>248</v>
+        <v>93</v>
       </c>
       <c r="Q36" s="1" t="s">
         <v>34</v>
@@ -5018,7 +5033,7 @@
         <v>34</v>
       </c>
       <c r="S36" s="1" t="s">
-        <v>249</v>
+        <v>94</v>
       </c>
       <c r="T36" s="1" t="s">
         <v>34</v>
@@ -5027,7 +5042,7 @@
         <v>34</v>
       </c>
       <c r="V36" s="1" t="s">
-        <v>250</v>
+        <v>95</v>
       </c>
       <c r="W36" s="1" t="s">
         <v>34</v>
@@ -5039,7 +5054,7 @@
         <v>40</v>
       </c>
       <c r="Z36" s="1" t="s">
-        <v>157</v>
+        <v>41</v>
       </c>
       <c r="AA36" s="1" t="s">
         <v>42</v>
@@ -5071,7 +5086,7 @@
         <v>14</v>
       </c>
       <c r="D37" s="2">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E37" s="1" t="s">
         <v>32</v>
@@ -5089,7 +5104,7 @@
         <v>34</v>
       </c>
       <c r="J37" s="1" t="s">
-        <v>226</v>
+        <v>246</v>
       </c>
       <c r="K37" s="1" t="s">
         <v>34</v>
@@ -5098,7 +5113,7 @@
         <v>34</v>
       </c>
       <c r="M37" s="1" t="s">
-        <v>227</v>
+        <v>247</v>
       </c>
       <c r="N37" s="1" t="s">
         <v>34</v>
@@ -5107,7 +5122,7 @@
         <v>34</v>
       </c>
       <c r="P37" s="1" t="s">
-        <v>228</v>
+        <v>248</v>
       </c>
       <c r="Q37" s="1" t="s">
         <v>34</v>
@@ -5116,7 +5131,7 @@
         <v>34</v>
       </c>
       <c r="S37" s="1" t="s">
-        <v>229</v>
+        <v>249</v>
       </c>
       <c r="T37" s="1" t="s">
         <v>34</v>
@@ -5125,7 +5140,7 @@
         <v>34</v>
       </c>
       <c r="V37" s="1" t="s">
-        <v>230</v>
+        <v>250</v>
       </c>
       <c r="W37" s="1" t="s">
         <v>34</v>
@@ -5137,7 +5152,7 @@
         <v>40</v>
       </c>
       <c r="Z37" s="1" t="s">
-        <v>53</v>
+        <v>157</v>
       </c>
       <c r="AA37" s="1" t="s">
         <v>42</v>
@@ -5169,7 +5184,7 @@
         <v>14</v>
       </c>
       <c r="D38" s="2">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E38" s="1" t="s">
         <v>32</v>
@@ -5187,7 +5202,7 @@
         <v>34</v>
       </c>
       <c r="J38" s="1" t="s">
-        <v>118</v>
+        <v>226</v>
       </c>
       <c r="K38" s="1" t="s">
         <v>34</v>
@@ -5196,7 +5211,7 @@
         <v>34</v>
       </c>
       <c r="M38" s="1" t="s">
-        <v>119</v>
+        <v>227</v>
       </c>
       <c r="N38" s="1" t="s">
         <v>34</v>
@@ -5205,7 +5220,7 @@
         <v>34</v>
       </c>
       <c r="P38" s="1" t="s">
-        <v>120</v>
+        <v>228</v>
       </c>
       <c r="Q38" s="1" t="s">
         <v>34</v>
@@ -5214,7 +5229,7 @@
         <v>34</v>
       </c>
       <c r="S38" s="1" t="s">
-        <v>121</v>
+        <v>229</v>
       </c>
       <c r="T38" s="1" t="s">
         <v>34</v>
@@ -5223,7 +5238,7 @@
         <v>34</v>
       </c>
       <c r="V38" s="1" t="s">
-        <v>122</v>
+        <v>230</v>
       </c>
       <c r="W38" s="1" t="s">
         <v>34</v>
@@ -5235,7 +5250,7 @@
         <v>40</v>
       </c>
       <c r="Z38" s="1" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="AA38" s="1" t="s">
         <v>42</v>
@@ -5267,7 +5282,7 @@
         <v>14</v>
       </c>
       <c r="D39" s="2">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E39" s="1" t="s">
         <v>32</v>
@@ -5285,7 +5300,7 @@
         <v>34</v>
       </c>
       <c r="J39" s="1" t="s">
-        <v>80</v>
+        <v>118</v>
       </c>
       <c r="K39" s="1" t="s">
         <v>34</v>
@@ -5294,7 +5309,7 @@
         <v>34</v>
       </c>
       <c r="M39" s="1" t="s">
-        <v>81</v>
+        <v>119</v>
       </c>
       <c r="N39" s="1" t="s">
         <v>34</v>
@@ -5303,7 +5318,7 @@
         <v>34</v>
       </c>
       <c r="P39" s="1" t="s">
-        <v>82</v>
+        <v>120</v>
       </c>
       <c r="Q39" s="1" t="s">
         <v>34</v>
@@ -5312,7 +5327,7 @@
         <v>34</v>
       </c>
       <c r="S39" s="1" t="s">
-        <v>83</v>
+        <v>121</v>
       </c>
       <c r="T39" s="1" t="s">
         <v>34</v>
@@ -5321,7 +5336,7 @@
         <v>34</v>
       </c>
       <c r="V39" s="1" t="s">
-        <v>84</v>
+        <v>122</v>
       </c>
       <c r="W39" s="1" t="s">
         <v>34</v>
@@ -5333,7 +5348,7 @@
         <v>40</v>
       </c>
       <c r="Z39" s="1" t="s">
-        <v>85</v>
+        <v>59</v>
       </c>
       <c r="AA39" s="1" t="s">
         <v>42</v>
@@ -5365,7 +5380,7 @@
         <v>14</v>
       </c>
       <c r="D40" s="2">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E40" s="1" t="s">
         <v>32</v>
@@ -5383,7 +5398,7 @@
         <v>34</v>
       </c>
       <c r="J40" s="1" t="s">
-        <v>291</v>
+        <v>80</v>
       </c>
       <c r="K40" s="1" t="s">
         <v>34</v>
@@ -5392,7 +5407,7 @@
         <v>34</v>
       </c>
       <c r="M40" s="1" t="s">
-        <v>292</v>
+        <v>81</v>
       </c>
       <c r="N40" s="1" t="s">
         <v>34</v>
@@ -5401,7 +5416,7 @@
         <v>34</v>
       </c>
       <c r="P40" s="1" t="s">
-        <v>293</v>
+        <v>82</v>
       </c>
       <c r="Q40" s="1" t="s">
         <v>34</v>
@@ -5410,7 +5425,7 @@
         <v>34</v>
       </c>
       <c r="S40" s="1" t="s">
-        <v>294</v>
+        <v>83</v>
       </c>
       <c r="T40" s="1" t="s">
         <v>34</v>
@@ -5419,7 +5434,7 @@
         <v>34</v>
       </c>
       <c r="V40" s="1" t="s">
-        <v>295</v>
+        <v>84</v>
       </c>
       <c r="W40" s="1" t="s">
         <v>34</v>
@@ -5431,7 +5446,7 @@
         <v>40</v>
       </c>
       <c r="Z40" s="1" t="s">
-        <v>157</v>
+        <v>85</v>
       </c>
       <c r="AA40" s="1" t="s">
         <v>42</v>
@@ -5463,7 +5478,7 @@
         <v>14</v>
       </c>
       <c r="D41" s="2">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E41" s="1" t="s">
         <v>32</v>
@@ -5481,7 +5496,7 @@
         <v>34</v>
       </c>
       <c r="J41" s="1" t="s">
-        <v>168</v>
+        <v>291</v>
       </c>
       <c r="K41" s="1" t="s">
         <v>34</v>
@@ -5490,7 +5505,7 @@
         <v>34</v>
       </c>
       <c r="M41" s="1" t="s">
-        <v>169</v>
+        <v>292</v>
       </c>
       <c r="N41" s="1" t="s">
         <v>34</v>
@@ -5499,7 +5514,7 @@
         <v>34</v>
       </c>
       <c r="P41" s="1" t="s">
-        <v>170</v>
+        <v>293</v>
       </c>
       <c r="Q41" s="1" t="s">
         <v>34</v>
@@ -5508,7 +5523,7 @@
         <v>34</v>
       </c>
       <c r="S41" s="1" t="s">
-        <v>171</v>
+        <v>294</v>
       </c>
       <c r="T41" s="1" t="s">
         <v>34</v>
@@ -5517,7 +5532,7 @@
         <v>34</v>
       </c>
       <c r="V41" s="1" t="s">
-        <v>172</v>
+        <v>295</v>
       </c>
       <c r="W41" s="1" t="s">
         <v>34</v>
@@ -5529,7 +5544,7 @@
         <v>40</v>
       </c>
       <c r="Z41" s="1" t="s">
-        <v>85</v>
+        <v>157</v>
       </c>
       <c r="AA41" s="1" t="s">
         <v>42</v>
@@ -5561,7 +5576,7 @@
         <v>14</v>
       </c>
       <c r="D42" s="2">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E42" s="1" t="s">
         <v>32</v>
@@ -5579,7 +5594,7 @@
         <v>34</v>
       </c>
       <c r="J42" s="1" t="s">
-        <v>65</v>
+        <v>168</v>
       </c>
       <c r="K42" s="1" t="s">
         <v>34</v>
@@ -5588,7 +5603,7 @@
         <v>34</v>
       </c>
       <c r="M42" s="1" t="s">
-        <v>66</v>
+        <v>169</v>
       </c>
       <c r="N42" s="1" t="s">
         <v>34</v>
@@ -5597,7 +5612,7 @@
         <v>34</v>
       </c>
       <c r="P42" s="1" t="s">
-        <v>60</v>
+        <v>170</v>
       </c>
       <c r="Q42" s="1" t="s">
         <v>34</v>
@@ -5606,7 +5621,7 @@
         <v>34</v>
       </c>
       <c r="S42" s="1" t="s">
-        <v>67</v>
+        <v>171</v>
       </c>
       <c r="T42" s="1" t="s">
         <v>34</v>
@@ -5615,7 +5630,7 @@
         <v>34</v>
       </c>
       <c r="V42" s="1" t="s">
-        <v>68</v>
+        <v>172</v>
       </c>
       <c r="W42" s="1" t="s">
         <v>34</v>
@@ -5627,7 +5642,7 @@
         <v>40</v>
       </c>
       <c r="Z42" s="1" t="s">
-        <v>41</v>
+        <v>85</v>
       </c>
       <c r="AA42" s="1" t="s">
         <v>42</v>
@@ -5659,7 +5674,7 @@
         <v>14</v>
       </c>
       <c r="D43" s="2">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E43" s="1" t="s">
         <v>32</v>
@@ -5677,7 +5692,7 @@
         <v>34</v>
       </c>
       <c r="J43" s="1" t="s">
-        <v>296</v>
+        <v>65</v>
       </c>
       <c r="K43" s="1" t="s">
         <v>34</v>
@@ -5686,7 +5701,7 @@
         <v>34</v>
       </c>
       <c r="M43" s="1" t="s">
-        <v>297</v>
+        <v>66</v>
       </c>
       <c r="N43" s="1" t="s">
         <v>34</v>
@@ -5695,7 +5710,7 @@
         <v>34</v>
       </c>
       <c r="P43" s="1" t="s">
-        <v>298</v>
+        <v>60</v>
       </c>
       <c r="Q43" s="1" t="s">
         <v>34</v>
@@ -5704,7 +5719,7 @@
         <v>34</v>
       </c>
       <c r="S43" s="1" t="s">
-        <v>299</v>
+        <v>67</v>
       </c>
       <c r="T43" s="1" t="s">
         <v>34</v>
@@ -5713,7 +5728,7 @@
         <v>34</v>
       </c>
       <c r="V43" s="1" t="s">
-        <v>300</v>
+        <v>68</v>
       </c>
       <c r="W43" s="1" t="s">
         <v>34</v>
@@ -5725,7 +5740,7 @@
         <v>40</v>
       </c>
       <c r="Z43" s="1" t="s">
-        <v>301</v>
+        <v>41</v>
       </c>
       <c r="AA43" s="1" t="s">
         <v>42</v>
@@ -5757,7 +5772,7 @@
         <v>14</v>
       </c>
       <c r="D44" s="2">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E44" s="1" t="s">
         <v>32</v>
@@ -5775,7 +5790,7 @@
         <v>34</v>
       </c>
       <c r="J44" s="1" t="s">
-        <v>184</v>
+        <v>296</v>
       </c>
       <c r="K44" s="1" t="s">
         <v>34</v>
@@ -5784,7 +5799,7 @@
         <v>34</v>
       </c>
       <c r="M44" s="1" t="s">
-        <v>185</v>
+        <v>297</v>
       </c>
       <c r="N44" s="1" t="s">
         <v>34</v>
@@ -5793,7 +5808,7 @@
         <v>34</v>
       </c>
       <c r="P44" s="1" t="s">
-        <v>186</v>
+        <v>298</v>
       </c>
       <c r="Q44" s="1" t="s">
         <v>34</v>
@@ -5802,7 +5817,7 @@
         <v>34</v>
       </c>
       <c r="S44" s="1" t="s">
-        <v>187</v>
+        <v>299</v>
       </c>
       <c r="T44" s="1" t="s">
         <v>34</v>
@@ -5811,7 +5826,7 @@
         <v>34</v>
       </c>
       <c r="V44" s="1" t="s">
-        <v>188</v>
+        <v>300</v>
       </c>
       <c r="W44" s="1" t="s">
         <v>34</v>
@@ -5823,7 +5838,7 @@
         <v>40</v>
       </c>
       <c r="Z44" s="1" t="s">
-        <v>101</v>
+        <v>301</v>
       </c>
       <c r="AA44" s="1" t="s">
         <v>42</v>
@@ -5855,7 +5870,7 @@
         <v>14</v>
       </c>
       <c r="D45" s="2">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E45" s="1" t="s">
         <v>32</v>
@@ -5873,7 +5888,7 @@
         <v>34</v>
       </c>
       <c r="J45" s="1" t="s">
-        <v>163</v>
+        <v>184</v>
       </c>
       <c r="K45" s="1" t="s">
         <v>34</v>
@@ -5882,7 +5897,7 @@
         <v>34</v>
       </c>
       <c r="M45" s="1" t="s">
-        <v>164</v>
+        <v>185</v>
       </c>
       <c r="N45" s="1" t="s">
         <v>34</v>
@@ -5891,7 +5906,7 @@
         <v>34</v>
       </c>
       <c r="P45" s="1" t="s">
-        <v>165</v>
+        <v>186</v>
       </c>
       <c r="Q45" s="1" t="s">
         <v>34</v>
@@ -5900,7 +5915,7 @@
         <v>34</v>
       </c>
       <c r="S45" s="1" t="s">
-        <v>166</v>
+        <v>187</v>
       </c>
       <c r="T45" s="1" t="s">
         <v>34</v>
@@ -5909,7 +5924,7 @@
         <v>34</v>
       </c>
       <c r="V45" s="1" t="s">
-        <v>167</v>
+        <v>188</v>
       </c>
       <c r="W45" s="1" t="s">
         <v>34</v>
@@ -5921,7 +5936,7 @@
         <v>40</v>
       </c>
       <c r="Z45" s="1" t="s">
-        <v>59</v>
+        <v>101</v>
       </c>
       <c r="AA45" s="1" t="s">
         <v>42</v>
@@ -5953,7 +5968,7 @@
         <v>14</v>
       </c>
       <c r="D46" s="2">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E46" s="1" t="s">
         <v>32</v>
@@ -5971,7 +5986,7 @@
         <v>34</v>
       </c>
       <c r="J46" s="1" t="s">
-        <v>276</v>
+        <v>163</v>
       </c>
       <c r="K46" s="1" t="s">
         <v>34</v>
@@ -5980,7 +5995,7 @@
         <v>34</v>
       </c>
       <c r="M46" s="1" t="s">
-        <v>277</v>
+        <v>164</v>
       </c>
       <c r="N46" s="1" t="s">
         <v>34</v>
@@ -5989,7 +6004,7 @@
         <v>34</v>
       </c>
       <c r="P46" s="1" t="s">
-        <v>278</v>
+        <v>165</v>
       </c>
       <c r="Q46" s="1" t="s">
         <v>34</v>
@@ -5998,7 +6013,7 @@
         <v>34</v>
       </c>
       <c r="S46" s="1" t="s">
-        <v>279</v>
+        <v>166</v>
       </c>
       <c r="T46" s="1" t="s">
         <v>34</v>
@@ -6007,7 +6022,7 @@
         <v>34</v>
       </c>
       <c r="V46" s="1" t="s">
-        <v>280</v>
+        <v>167</v>
       </c>
       <c r="W46" s="1" t="s">
         <v>34</v>
@@ -6019,7 +6034,7 @@
         <v>40</v>
       </c>
       <c r="Z46" s="1" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="AA46" s="1" t="s">
         <v>42</v>
@@ -6051,7 +6066,7 @@
         <v>14</v>
       </c>
       <c r="D47" s="2">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E47" s="1" t="s">
         <v>32</v>
@@ -6069,7 +6084,7 @@
         <v>34</v>
       </c>
       <c r="J47" s="1" t="s">
-        <v>173</v>
+        <v>276</v>
       </c>
       <c r="K47" s="1" t="s">
         <v>34</v>
@@ -6078,7 +6093,7 @@
         <v>34</v>
       </c>
       <c r="M47" s="1" t="s">
-        <v>174</v>
+        <v>277</v>
       </c>
       <c r="N47" s="1" t="s">
         <v>34</v>
@@ -6087,7 +6102,7 @@
         <v>34</v>
       </c>
       <c r="P47" s="1" t="s">
-        <v>175</v>
+        <v>278</v>
       </c>
       <c r="Q47" s="1" t="s">
         <v>34</v>
@@ -6096,7 +6111,7 @@
         <v>34</v>
       </c>
       <c r="S47" s="1" t="s">
-        <v>176</v>
+        <v>279</v>
       </c>
       <c r="T47" s="1" t="s">
         <v>34</v>
@@ -6105,7 +6120,7 @@
         <v>34</v>
       </c>
       <c r="V47" s="1" t="s">
-        <v>177</v>
+        <v>280</v>
       </c>
       <c r="W47" s="1" t="s">
         <v>34</v>
@@ -6117,7 +6132,7 @@
         <v>40</v>
       </c>
       <c r="Z47" s="1" t="s">
-        <v>41</v>
+        <v>53</v>
       </c>
       <c r="AA47" s="1" t="s">
         <v>42</v>
@@ -6149,7 +6164,7 @@
         <v>14</v>
       </c>
       <c r="D48" s="2">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E48" s="1" t="s">
         <v>32</v>
@@ -6167,7 +6182,7 @@
         <v>34</v>
       </c>
       <c r="J48" s="1" t="s">
-        <v>133</v>
+        <v>173</v>
       </c>
       <c r="K48" s="1" t="s">
         <v>34</v>
@@ -6176,7 +6191,7 @@
         <v>34</v>
       </c>
       <c r="M48" s="1" t="s">
-        <v>134</v>
+        <v>174</v>
       </c>
       <c r="N48" s="1" t="s">
         <v>34</v>
@@ -6185,7 +6200,7 @@
         <v>34</v>
       </c>
       <c r="P48" s="1" t="s">
-        <v>135</v>
+        <v>175</v>
       </c>
       <c r="Q48" s="1" t="s">
         <v>34</v>
@@ -6194,7 +6209,7 @@
         <v>34</v>
       </c>
       <c r="S48" s="1" t="s">
-        <v>136</v>
+        <v>176</v>
       </c>
       <c r="T48" s="1" t="s">
         <v>34</v>
@@ -6203,7 +6218,7 @@
         <v>34</v>
       </c>
       <c r="V48" s="1" t="s">
-        <v>137</v>
+        <v>177</v>
       </c>
       <c r="W48" s="1" t="s">
         <v>34</v>
@@ -6215,7 +6230,7 @@
         <v>40</v>
       </c>
       <c r="Z48" s="1" t="s">
-        <v>101</v>
+        <v>41</v>
       </c>
       <c r="AA48" s="1" t="s">
         <v>42</v>
@@ -6247,7 +6262,7 @@
         <v>14</v>
       </c>
       <c r="D49" s="2">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E49" s="1" t="s">
         <v>32</v>
@@ -6265,7 +6280,7 @@
         <v>34</v>
       </c>
       <c r="J49" s="1" t="s">
-        <v>266</v>
+        <v>133</v>
       </c>
       <c r="K49" s="1" t="s">
         <v>34</v>
@@ -6274,7 +6289,7 @@
         <v>34</v>
       </c>
       <c r="M49" s="1" t="s">
-        <v>267</v>
+        <v>134</v>
       </c>
       <c r="N49" s="1" t="s">
         <v>34</v>
@@ -6283,7 +6298,7 @@
         <v>34</v>
       </c>
       <c r="P49" s="1" t="s">
-        <v>268</v>
+        <v>135</v>
       </c>
       <c r="Q49" s="1" t="s">
         <v>34</v>
@@ -6292,7 +6307,7 @@
         <v>34</v>
       </c>
       <c r="S49" s="1" t="s">
-        <v>269</v>
+        <v>136</v>
       </c>
       <c r="T49" s="1" t="s">
         <v>34</v>
@@ -6301,7 +6316,7 @@
         <v>34</v>
       </c>
       <c r="V49" s="1" t="s">
-        <v>270</v>
+        <v>137</v>
       </c>
       <c r="W49" s="1" t="s">
         <v>34</v>
@@ -6313,7 +6328,7 @@
         <v>40</v>
       </c>
       <c r="Z49" s="1" t="s">
-        <v>59</v>
+        <v>101</v>
       </c>
       <c r="AA49" s="1" t="s">
         <v>42</v>
@@ -6345,7 +6360,7 @@
         <v>14</v>
       </c>
       <c r="D50" s="2">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E50" s="1" t="s">
         <v>32</v>
@@ -6363,7 +6378,7 @@
         <v>34</v>
       </c>
       <c r="J50" s="1" t="s">
-        <v>281</v>
+        <v>266</v>
       </c>
       <c r="K50" s="1" t="s">
         <v>34</v>
@@ -6372,7 +6387,7 @@
         <v>34</v>
       </c>
       <c r="M50" s="1" t="s">
-        <v>282</v>
+        <v>267</v>
       </c>
       <c r="N50" s="1" t="s">
         <v>34</v>
@@ -6381,7 +6396,7 @@
         <v>34</v>
       </c>
       <c r="P50" s="1" t="s">
-        <v>283</v>
+        <v>268</v>
       </c>
       <c r="Q50" s="1" t="s">
         <v>34</v>
@@ -6390,7 +6405,7 @@
         <v>34</v>
       </c>
       <c r="S50" s="1" t="s">
-        <v>284</v>
+        <v>269</v>
       </c>
       <c r="T50" s="1" t="s">
         <v>34</v>
@@ -6399,7 +6414,7 @@
         <v>34</v>
       </c>
       <c r="V50" s="1" t="s">
-        <v>285</v>
+        <v>270</v>
       </c>
       <c r="W50" s="1" t="s">
         <v>34</v>
@@ -6411,7 +6426,7 @@
         <v>40</v>
       </c>
       <c r="Z50" s="1" t="s">
-        <v>85</v>
+        <v>59</v>
       </c>
       <c r="AA50" s="1" t="s">
         <v>42</v>
@@ -6443,7 +6458,7 @@
         <v>14</v>
       </c>
       <c r="D51" s="2">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E51" s="1" t="s">
         <v>32</v>
@@ -6461,7 +6476,7 @@
         <v>34</v>
       </c>
       <c r="J51" s="1" t="s">
-        <v>112</v>
+        <v>281</v>
       </c>
       <c r="K51" s="1" t="s">
         <v>34</v>
@@ -6470,7 +6485,7 @@
         <v>34</v>
       </c>
       <c r="M51" s="1" t="s">
-        <v>113</v>
+        <v>282</v>
       </c>
       <c r="N51" s="1" t="s">
         <v>34</v>
@@ -6479,7 +6494,7 @@
         <v>34</v>
       </c>
       <c r="P51" s="1" t="s">
-        <v>114</v>
+        <v>283</v>
       </c>
       <c r="Q51" s="1" t="s">
         <v>34</v>
@@ -6488,7 +6503,7 @@
         <v>34</v>
       </c>
       <c r="S51" s="1" t="s">
-        <v>115</v>
+        <v>284</v>
       </c>
       <c r="T51" s="1" t="s">
         <v>34</v>
@@ -6497,7 +6512,7 @@
         <v>34</v>
       </c>
       <c r="V51" s="1" t="s">
-        <v>116</v>
+        <v>285</v>
       </c>
       <c r="W51" s="1" t="s">
         <v>34</v>
@@ -6509,7 +6524,7 @@
         <v>40</v>
       </c>
       <c r="Z51" s="1" t="s">
-        <v>117</v>
+        <v>85</v>
       </c>
       <c r="AA51" s="1" t="s">
         <v>42</v>
@@ -6541,7 +6556,7 @@
         <v>14</v>
       </c>
       <c r="D52" s="2">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E52" s="1" t="s">
         <v>32</v>
@@ -6559,7 +6574,7 @@
         <v>34</v>
       </c>
       <c r="J52" s="1" t="s">
-        <v>86</v>
+        <v>112</v>
       </c>
       <c r="K52" s="1" t="s">
         <v>34</v>
@@ -6568,7 +6583,7 @@
         <v>34</v>
       </c>
       <c r="M52" s="1" t="s">
-        <v>87</v>
+        <v>113</v>
       </c>
       <c r="N52" s="1" t="s">
         <v>34</v>
@@ -6577,7 +6592,7 @@
         <v>34</v>
       </c>
       <c r="P52" s="1" t="s">
-        <v>88</v>
+        <v>114</v>
       </c>
       <c r="Q52" s="1" t="s">
         <v>34</v>
@@ -6586,7 +6601,7 @@
         <v>34</v>
       </c>
       <c r="S52" s="1" t="s">
-        <v>89</v>
+        <v>115</v>
       </c>
       <c r="T52" s="1" t="s">
         <v>34</v>
@@ -6595,7 +6610,7 @@
         <v>34</v>
       </c>
       <c r="V52" s="1" t="s">
-        <v>90</v>
+        <v>116</v>
       </c>
       <c r="W52" s="1" t="s">
         <v>34</v>
@@ -6607,7 +6622,7 @@
         <v>40</v>
       </c>
       <c r="Z52" s="1" t="s">
-        <v>53</v>
+        <v>117</v>
       </c>
       <c r="AA52" s="1" t="s">
         <v>42</v>
@@ -6633,13 +6648,13 @@
         <v>358</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>307</v>
+        <v>31</v>
       </c>
       <c r="C53" s="2">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="D53" s="2">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="E53" s="1" t="s">
         <v>32</v>
@@ -6657,7 +6672,7 @@
         <v>34</v>
       </c>
       <c r="J53" s="1" t="s">
-        <v>347</v>
+        <v>86</v>
       </c>
       <c r="K53" s="1" t="s">
         <v>34</v>
@@ -6666,7 +6681,7 @@
         <v>34</v>
       </c>
       <c r="M53" s="1" t="s">
-        <v>348</v>
+        <v>87</v>
       </c>
       <c r="N53" s="1" t="s">
         <v>34</v>
@@ -6675,7 +6690,7 @@
         <v>34</v>
       </c>
       <c r="P53" s="1" t="s">
-        <v>349</v>
+        <v>88</v>
       </c>
       <c r="Q53" s="1" t="s">
         <v>34</v>
@@ -6684,7 +6699,7 @@
         <v>34</v>
       </c>
       <c r="S53" s="1" t="s">
-        <v>350</v>
+        <v>89</v>
       </c>
       <c r="T53" s="1" t="s">
         <v>34</v>
@@ -6693,7 +6708,7 @@
         <v>34</v>
       </c>
       <c r="V53" s="1" t="s">
-        <v>351</v>
+        <v>90</v>
       </c>
       <c r="W53" s="1" t="s">
         <v>34</v>
@@ -6705,7 +6720,7 @@
         <v>40</v>
       </c>
       <c r="Z53" s="1" t="s">
-        <v>117</v>
+        <v>53</v>
       </c>
       <c r="AA53" s="1" t="s">
         <v>42</v>
@@ -6737,7 +6752,7 @@
         <v>17</v>
       </c>
       <c r="D54" s="2">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="E54" s="1" t="s">
         <v>32</v>
@@ -6755,7 +6770,7 @@
         <v>34</v>
       </c>
       <c r="J54" s="1" t="s">
-        <v>342</v>
+        <v>347</v>
       </c>
       <c r="K54" s="1" t="s">
         <v>34</v>
@@ -6764,7 +6779,7 @@
         <v>34</v>
       </c>
       <c r="M54" s="1" t="s">
-        <v>343</v>
+        <v>348</v>
       </c>
       <c r="N54" s="1" t="s">
         <v>34</v>
@@ -6773,7 +6788,7 @@
         <v>34</v>
       </c>
       <c r="P54" s="1" t="s">
-        <v>344</v>
+        <v>349</v>
       </c>
       <c r="Q54" s="1" t="s">
         <v>34</v>
@@ -6782,7 +6797,7 @@
         <v>34</v>
       </c>
       <c r="S54" s="1" t="s">
-        <v>345</v>
+        <v>350</v>
       </c>
       <c r="T54" s="1" t="s">
         <v>34</v>
@@ -6791,7 +6806,7 @@
         <v>34</v>
       </c>
       <c r="V54" s="1" t="s">
-        <v>346</v>
+        <v>351</v>
       </c>
       <c r="W54" s="1" t="s">
         <v>34</v>
@@ -6835,7 +6850,7 @@
         <v>17</v>
       </c>
       <c r="D55" s="2">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E55" s="1" t="s">
         <v>32</v>
@@ -6853,7 +6868,7 @@
         <v>34</v>
       </c>
       <c r="J55" s="1" t="s">
-        <v>313</v>
+        <v>342</v>
       </c>
       <c r="K55" s="1" t="s">
         <v>34</v>
@@ -6862,7 +6877,7 @@
         <v>34</v>
       </c>
       <c r="M55" s="1" t="s">
-        <v>314</v>
+        <v>343</v>
       </c>
       <c r="N55" s="1" t="s">
         <v>34</v>
@@ -6871,7 +6886,7 @@
         <v>34</v>
       </c>
       <c r="P55" s="1" t="s">
-        <v>315</v>
+        <v>344</v>
       </c>
       <c r="Q55" s="1" t="s">
         <v>34</v>
@@ -6880,7 +6895,7 @@
         <v>34</v>
       </c>
       <c r="S55" s="1" t="s">
-        <v>316</v>
+        <v>345</v>
       </c>
       <c r="T55" s="1" t="s">
         <v>34</v>
@@ -6889,7 +6904,7 @@
         <v>34</v>
       </c>
       <c r="V55" s="1" t="s">
-        <v>317</v>
+        <v>346</v>
       </c>
       <c r="W55" s="1" t="s">
         <v>34</v>
@@ -6933,7 +6948,7 @@
         <v>17</v>
       </c>
       <c r="D56" s="2">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="E56" s="1" t="s">
         <v>32</v>
@@ -6951,7 +6966,7 @@
         <v>34</v>
       </c>
       <c r="J56" s="1" t="s">
-        <v>323</v>
+        <v>313</v>
       </c>
       <c r="K56" s="1" t="s">
         <v>34</v>
@@ -6960,7 +6975,7 @@
         <v>34</v>
       </c>
       <c r="M56" s="1" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="N56" s="1" t="s">
         <v>34</v>
@@ -6969,7 +6984,7 @@
         <v>34</v>
       </c>
       <c r="P56" s="1" t="s">
-        <v>324</v>
+        <v>315</v>
       </c>
       <c r="Q56" s="1" t="s">
         <v>34</v>
@@ -6978,7 +6993,7 @@
         <v>34</v>
       </c>
       <c r="S56" s="1" t="s">
-        <v>325</v>
+        <v>316</v>
       </c>
       <c r="T56" s="1" t="s">
         <v>34</v>
@@ -6987,7 +7002,7 @@
         <v>34</v>
       </c>
       <c r="V56" s="1" t="s">
-        <v>326</v>
+        <v>317</v>
       </c>
       <c r="W56" s="1" t="s">
         <v>34</v>
@@ -7031,7 +7046,7 @@
         <v>17</v>
       </c>
       <c r="D57" s="2">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E57" s="1" t="s">
         <v>32</v>
@@ -7049,7 +7064,7 @@
         <v>34</v>
       </c>
       <c r="J57" s="1" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
       <c r="K57" s="1" t="s">
         <v>34</v>
@@ -7058,7 +7073,7 @@
         <v>34</v>
       </c>
       <c r="M57" s="1" t="s">
-        <v>328</v>
+        <v>313</v>
       </c>
       <c r="N57" s="1" t="s">
         <v>34</v>
@@ -7067,7 +7082,7 @@
         <v>34</v>
       </c>
       <c r="P57" s="1" t="s">
-        <v>329</v>
+        <v>324</v>
       </c>
       <c r="Q57" s="1" t="s">
         <v>34</v>
@@ -7076,7 +7091,7 @@
         <v>34</v>
       </c>
       <c r="S57" s="1" t="s">
-        <v>330</v>
+        <v>325</v>
       </c>
       <c r="T57" s="1" t="s">
         <v>34</v>
@@ -7085,7 +7100,7 @@
         <v>34</v>
       </c>
       <c r="V57" s="1" t="s">
-        <v>331</v>
+        <v>326</v>
       </c>
       <c r="W57" s="1" t="s">
         <v>34</v>
@@ -7129,7 +7144,7 @@
         <v>17</v>
       </c>
       <c r="D58" s="2">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E58" s="1" t="s">
         <v>32</v>
@@ -7147,7 +7162,7 @@
         <v>34</v>
       </c>
       <c r="J58" s="1" t="s">
-        <v>308</v>
+        <v>327</v>
       </c>
       <c r="K58" s="1" t="s">
         <v>34</v>
@@ -7156,7 +7171,7 @@
         <v>34</v>
       </c>
       <c r="M58" s="1" t="s">
-        <v>309</v>
+        <v>328</v>
       </c>
       <c r="N58" s="1" t="s">
         <v>34</v>
@@ -7165,7 +7180,7 @@
         <v>34</v>
       </c>
       <c r="P58" s="1" t="s">
-        <v>310</v>
+        <v>329</v>
       </c>
       <c r="Q58" s="1" t="s">
         <v>34</v>
@@ -7174,7 +7189,7 @@
         <v>34</v>
       </c>
       <c r="S58" s="1" t="s">
-        <v>311</v>
+        <v>330</v>
       </c>
       <c r="T58" s="1" t="s">
         <v>34</v>
@@ -7183,7 +7198,7 @@
         <v>34</v>
       </c>
       <c r="V58" s="1" t="s">
-        <v>312</v>
+        <v>331</v>
       </c>
       <c r="W58" s="1" t="s">
         <v>34</v>
@@ -7227,7 +7242,7 @@
         <v>17</v>
       </c>
       <c r="D59" s="2">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E59" s="1" t="s">
         <v>32</v>
@@ -7245,7 +7260,7 @@
         <v>34</v>
       </c>
       <c r="J59" s="1" t="s">
-        <v>337</v>
+        <v>308</v>
       </c>
       <c r="K59" s="1" t="s">
         <v>34</v>
@@ -7254,7 +7269,7 @@
         <v>34</v>
       </c>
       <c r="M59" s="1" t="s">
-        <v>338</v>
+        <v>309</v>
       </c>
       <c r="N59" s="1" t="s">
         <v>34</v>
@@ -7263,7 +7278,7 @@
         <v>34</v>
       </c>
       <c r="P59" s="1" t="s">
-        <v>339</v>
+        <v>310</v>
       </c>
       <c r="Q59" s="1" t="s">
         <v>34</v>
@@ -7272,7 +7287,7 @@
         <v>34</v>
       </c>
       <c r="S59" s="1" t="s">
-        <v>340</v>
+        <v>311</v>
       </c>
       <c r="T59" s="1" t="s">
         <v>34</v>
@@ -7281,7 +7296,7 @@
         <v>34</v>
       </c>
       <c r="V59" s="1" t="s">
-        <v>341</v>
+        <v>312</v>
       </c>
       <c r="W59" s="1" t="s">
         <v>34</v>
@@ -7325,7 +7340,7 @@
         <v>17</v>
       </c>
       <c r="D60" s="2">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E60" s="1" t="s">
         <v>32</v>
@@ -7343,7 +7358,7 @@
         <v>34</v>
       </c>
       <c r="J60" s="1" t="s">
-        <v>332</v>
+        <v>337</v>
       </c>
       <c r="K60" s="1" t="s">
         <v>34</v>
@@ -7352,7 +7367,7 @@
         <v>34</v>
       </c>
       <c r="M60" s="1" t="s">
-        <v>333</v>
+        <v>338</v>
       </c>
       <c r="N60" s="1" t="s">
         <v>34</v>
@@ -7361,7 +7376,7 @@
         <v>34</v>
       </c>
       <c r="P60" s="1" t="s">
-        <v>334</v>
+        <v>339</v>
       </c>
       <c r="Q60" s="1" t="s">
         <v>34</v>
@@ -7370,7 +7385,7 @@
         <v>34</v>
       </c>
       <c r="S60" s="1" t="s">
-        <v>335</v>
+        <v>340</v>
       </c>
       <c r="T60" s="1" t="s">
         <v>34</v>
@@ -7379,7 +7394,7 @@
         <v>34</v>
       </c>
       <c r="V60" s="1" t="s">
-        <v>336</v>
+        <v>341</v>
       </c>
       <c r="W60" s="1" t="s">
         <v>34</v>
@@ -7423,7 +7438,7 @@
         <v>17</v>
       </c>
       <c r="D61" s="2">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E61" s="1" t="s">
         <v>32</v>
@@ -7441,7 +7456,7 @@
         <v>34</v>
       </c>
       <c r="J61" s="1" t="s">
-        <v>352</v>
+        <v>332</v>
       </c>
       <c r="K61" s="1" t="s">
         <v>34</v>
@@ -7450,7 +7465,7 @@
         <v>34</v>
       </c>
       <c r="M61" s="1" t="s">
-        <v>353</v>
+        <v>333</v>
       </c>
       <c r="N61" s="1" t="s">
         <v>34</v>
@@ -7459,7 +7474,7 @@
         <v>34</v>
       </c>
       <c r="P61" s="1" t="s">
-        <v>354</v>
+        <v>334</v>
       </c>
       <c r="Q61" s="1" t="s">
         <v>34</v>
@@ -7468,7 +7483,7 @@
         <v>34</v>
       </c>
       <c r="S61" s="1" t="s">
-        <v>355</v>
+        <v>335</v>
       </c>
       <c r="T61" s="1" t="s">
         <v>34</v>
@@ -7477,7 +7492,7 @@
         <v>34</v>
       </c>
       <c r="V61" s="1" t="s">
-        <v>356</v>
+        <v>336</v>
       </c>
       <c r="W61" s="1" t="s">
         <v>34</v>
@@ -7521,7 +7536,7 @@
         <v>17</v>
       </c>
       <c r="D62" s="2">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="E62" s="1" t="s">
         <v>32</v>
@@ -7539,7 +7554,7 @@
         <v>34</v>
       </c>
       <c r="J62" s="1" t="s">
-        <v>318</v>
+        <v>352</v>
       </c>
       <c r="K62" s="1" t="s">
         <v>34</v>
@@ -7548,7 +7563,7 @@
         <v>34</v>
       </c>
       <c r="M62" s="1" t="s">
-        <v>319</v>
+        <v>353</v>
       </c>
       <c r="N62" s="1" t="s">
         <v>34</v>
@@ -7557,7 +7572,7 @@
         <v>34</v>
       </c>
       <c r="P62" s="1" t="s">
-        <v>320</v>
+        <v>354</v>
       </c>
       <c r="Q62" s="1" t="s">
         <v>34</v>
@@ -7566,7 +7581,7 @@
         <v>34</v>
       </c>
       <c r="S62" s="1" t="s">
-        <v>321</v>
+        <v>355</v>
       </c>
       <c r="T62" s="1" t="s">
         <v>34</v>
@@ -7575,7 +7590,7 @@
         <v>34</v>
       </c>
       <c r="V62" s="1" t="s">
-        <v>322</v>
+        <v>356</v>
       </c>
       <c r="W62" s="1" t="s">
         <v>34</v>
@@ -7605,6 +7620,104 @@
         <v>46</v>
       </c>
       <c r="AF62" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="63" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A63" s="1" t="s">
+        <v>358</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>307</v>
+      </c>
+      <c r="C63" s="2">
+        <v>17</v>
+      </c>
+      <c r="D63" s="2">
+        <v>27</v>
+      </c>
+      <c r="E63" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F63" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="G63" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="H63" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="I63" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="J63" s="1" t="s">
+        <v>318</v>
+      </c>
+      <c r="K63" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="L63" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="M63" s="1" t="s">
+        <v>319</v>
+      </c>
+      <c r="N63" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="O63" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="P63" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="Q63" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="R63" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="S63" s="1" t="s">
+        <v>321</v>
+      </c>
+      <c r="T63" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="U63" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="V63" s="1" t="s">
+        <v>322</v>
+      </c>
+      <c r="W63" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="X63" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="Y63" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="Z63" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AA63" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AB63" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AC63" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AD63" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AE63" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AF63" s="1" t="s">
         <v>47</v>
       </c>
     </row>

</xml_diff>

<commit_message>
[SPONGE] fixing search of frames not present in raw data
</commit_message>
<xml_diff>
--- a/covid_dashboard/data/db_contacts.xlsx
+++ b/covid_dashboard/data/db_contacts.xlsx
@@ -1189,7 +1189,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1199,6 +1199,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1215,13 +1221,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="1" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1508,8 +1517,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AF63"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="V15" sqref="V15"/>
+    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="F46" sqref="F46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6741,983 +6750,983 @@
         <v>47</v>
       </c>
     </row>
-    <row r="54" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A54" s="1" t="s">
+    <row r="54" spans="1:32" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="6" t="s">
         <v>358</v>
       </c>
-      <c r="B54" s="1" t="s">
+      <c r="B54" s="6" t="s">
         <v>307</v>
       </c>
-      <c r="C54" s="2">
+      <c r="C54" s="7">
         <v>17</v>
       </c>
-      <c r="D54" s="2">
+      <c r="D54" s="7">
         <v>0</v>
       </c>
-      <c r="E54" s="1" t="s">
+      <c r="E54" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="F54" s="1" t="s">
+      <c r="F54" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="G54" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="H54" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="I54" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="J54" s="1" t="s">
+      <c r="G54" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="H54" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="I54" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="J54" s="6" t="s">
         <v>347</v>
       </c>
-      <c r="K54" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="L54" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="M54" s="1" t="s">
+      <c r="K54" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="L54" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="M54" s="6" t="s">
         <v>348</v>
       </c>
-      <c r="N54" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="O54" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="P54" s="1" t="s">
+      <c r="N54" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="O54" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="P54" s="6" t="s">
         <v>349</v>
       </c>
-      <c r="Q54" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="R54" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="S54" s="1" t="s">
+      <c r="Q54" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="R54" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="S54" s="6" t="s">
         <v>350</v>
       </c>
-      <c r="T54" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="U54" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="V54" s="1" t="s">
+      <c r="T54" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="U54" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="V54" s="6" t="s">
         <v>351</v>
       </c>
-      <c r="W54" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="X54" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="Y54" s="1" t="s">
+      <c r="W54" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="X54" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="Y54" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="Z54" s="1" t="s">
+      <c r="Z54" s="6" t="s">
         <v>117</v>
       </c>
-      <c r="AA54" s="1" t="s">
+      <c r="AA54" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="AB54" s="1" t="s">
+      <c r="AB54" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="AC54" s="1" t="s">
+      <c r="AC54" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="AD54" s="1" t="s">
+      <c r="AD54" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="AE54" s="1" t="s">
+      <c r="AE54" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="AF54" s="1" t="s">
+      <c r="AF54" s="6" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="55" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A55" s="1" t="s">
+    <row r="55" spans="1:32" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="6" t="s">
         <v>358</v>
       </c>
-      <c r="B55" s="1" t="s">
+      <c r="B55" s="6" t="s">
         <v>307</v>
       </c>
-      <c r="C55" s="2">
+      <c r="C55" s="7">
         <v>17</v>
       </c>
-      <c r="D55" s="2">
+      <c r="D55" s="7">
         <v>7</v>
       </c>
-      <c r="E55" s="1" t="s">
+      <c r="E55" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="F55" s="1" t="s">
+      <c r="F55" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="G55" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="H55" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="I55" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="J55" s="1" t="s">
+      <c r="G55" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="H55" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="I55" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="J55" s="6" t="s">
         <v>342</v>
       </c>
-      <c r="K55" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="L55" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="M55" s="1" t="s">
+      <c r="K55" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="L55" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="M55" s="6" t="s">
         <v>343</v>
       </c>
-      <c r="N55" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="O55" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="P55" s="1" t="s">
+      <c r="N55" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="O55" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="P55" s="6" t="s">
         <v>344</v>
       </c>
-      <c r="Q55" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="R55" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="S55" s="1" t="s">
+      <c r="Q55" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="R55" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="S55" s="6" t="s">
         <v>345</v>
       </c>
-      <c r="T55" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="U55" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="V55" s="1" t="s">
+      <c r="T55" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="U55" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="V55" s="6" t="s">
         <v>346</v>
       </c>
-      <c r="W55" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="X55" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="Y55" s="1" t="s">
+      <c r="W55" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="X55" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="Y55" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="Z55" s="1" t="s">
+      <c r="Z55" s="6" t="s">
         <v>117</v>
       </c>
-      <c r="AA55" s="1" t="s">
+      <c r="AA55" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="AB55" s="1" t="s">
+      <c r="AB55" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="AC55" s="1" t="s">
+      <c r="AC55" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="AD55" s="1" t="s">
+      <c r="AD55" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="AE55" s="1" t="s">
+      <c r="AE55" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="AF55" s="1" t="s">
+      <c r="AF55" s="6" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="56" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A56" s="1" t="s">
+    <row r="56" spans="1:32" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="6" t="s">
         <v>358</v>
       </c>
-      <c r="B56" s="1" t="s">
+      <c r="B56" s="6" t="s">
         <v>307</v>
       </c>
-      <c r="C56" s="2">
+      <c r="C56" s="7">
         <v>17</v>
       </c>
-      <c r="D56" s="2">
+      <c r="D56" s="7">
         <v>8</v>
       </c>
-      <c r="E56" s="1" t="s">
+      <c r="E56" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="F56" s="1" t="s">
+      <c r="F56" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="G56" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="H56" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="I56" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="J56" s="1" t="s">
+      <c r="G56" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="H56" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="I56" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="J56" s="6" t="s">
         <v>313</v>
       </c>
-      <c r="K56" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="L56" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="M56" s="1" t="s">
+      <c r="K56" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="L56" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="M56" s="6" t="s">
         <v>314</v>
       </c>
-      <c r="N56" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="O56" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="P56" s="1" t="s">
+      <c r="N56" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="O56" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="P56" s="6" t="s">
         <v>315</v>
       </c>
-      <c r="Q56" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="R56" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="S56" s="1" t="s">
+      <c r="Q56" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="R56" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="S56" s="6" t="s">
         <v>316</v>
       </c>
-      <c r="T56" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="U56" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="V56" s="1" t="s">
+      <c r="T56" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="U56" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="V56" s="6" t="s">
         <v>317</v>
       </c>
-      <c r="W56" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="X56" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="Y56" s="1" t="s">
+      <c r="W56" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="X56" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="Y56" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="Z56" s="1" t="s">
+      <c r="Z56" s="6" t="s">
         <v>117</v>
       </c>
-      <c r="AA56" s="1" t="s">
+      <c r="AA56" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="AB56" s="1" t="s">
+      <c r="AB56" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="AC56" s="1" t="s">
+      <c r="AC56" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="AD56" s="1" t="s">
+      <c r="AD56" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="AE56" s="1" t="s">
+      <c r="AE56" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="AF56" s="1" t="s">
+      <c r="AF56" s="6" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="57" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A57" s="1" t="s">
+    <row r="57" spans="1:32" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="6" t="s">
         <v>358</v>
       </c>
-      <c r="B57" s="1" t="s">
+      <c r="B57" s="6" t="s">
         <v>307</v>
       </c>
-      <c r="C57" s="2">
+      <c r="C57" s="7">
         <v>17</v>
       </c>
-      <c r="D57" s="2">
+      <c r="D57" s="7">
         <v>15</v>
       </c>
-      <c r="E57" s="1" t="s">
+      <c r="E57" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="F57" s="1" t="s">
+      <c r="F57" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="G57" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="H57" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="I57" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="J57" s="1" t="s">
+      <c r="G57" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="H57" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="I57" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="J57" s="6" t="s">
         <v>323</v>
       </c>
-      <c r="K57" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="L57" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="M57" s="1" t="s">
+      <c r="K57" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="L57" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="M57" s="6" t="s">
         <v>313</v>
       </c>
-      <c r="N57" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="O57" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="P57" s="1" t="s">
+      <c r="N57" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="O57" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="P57" s="6" t="s">
         <v>324</v>
       </c>
-      <c r="Q57" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="R57" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="S57" s="1" t="s">
+      <c r="Q57" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="R57" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="S57" s="6" t="s">
         <v>325</v>
       </c>
-      <c r="T57" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="U57" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="V57" s="1" t="s">
+      <c r="T57" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="U57" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="V57" s="6" t="s">
         <v>326</v>
       </c>
-      <c r="W57" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="X57" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="Y57" s="1" t="s">
+      <c r="W57" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="X57" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="Y57" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="Z57" s="1" t="s">
+      <c r="Z57" s="6" t="s">
         <v>117</v>
       </c>
-      <c r="AA57" s="1" t="s">
+      <c r="AA57" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="AB57" s="1" t="s">
+      <c r="AB57" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="AC57" s="1" t="s">
+      <c r="AC57" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="AD57" s="1" t="s">
+      <c r="AD57" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="AE57" s="1" t="s">
+      <c r="AE57" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="AF57" s="1" t="s">
+      <c r="AF57" s="6" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="58" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A58" s="1" t="s">
+    <row r="58" spans="1:32" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A58" s="6" t="s">
         <v>358</v>
       </c>
-      <c r="B58" s="1" t="s">
+      <c r="B58" s="6" t="s">
         <v>307</v>
       </c>
-      <c r="C58" s="2">
+      <c r="C58" s="7">
         <v>17</v>
       </c>
-      <c r="D58" s="2">
+      <c r="D58" s="7">
         <v>16</v>
       </c>
-      <c r="E58" s="1" t="s">
+      <c r="E58" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="F58" s="1" t="s">
+      <c r="F58" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="G58" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="H58" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="I58" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="J58" s="1" t="s">
+      <c r="G58" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="H58" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="I58" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="J58" s="6" t="s">
         <v>327</v>
       </c>
-      <c r="K58" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="L58" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="M58" s="1" t="s">
+      <c r="K58" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="L58" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="M58" s="6" t="s">
         <v>328</v>
       </c>
-      <c r="N58" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="O58" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="P58" s="1" t="s">
+      <c r="N58" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="O58" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="P58" s="6" t="s">
         <v>329</v>
       </c>
-      <c r="Q58" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="R58" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="S58" s="1" t="s">
+      <c r="Q58" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="R58" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="S58" s="6" t="s">
         <v>330</v>
       </c>
-      <c r="T58" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="U58" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="V58" s="1" t="s">
+      <c r="T58" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="U58" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="V58" s="6" t="s">
         <v>331</v>
       </c>
-      <c r="W58" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="X58" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="Y58" s="1" t="s">
+      <c r="W58" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="X58" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="Y58" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="Z58" s="1" t="s">
+      <c r="Z58" s="6" t="s">
         <v>117</v>
       </c>
-      <c r="AA58" s="1" t="s">
+      <c r="AA58" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="AB58" s="1" t="s">
+      <c r="AB58" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="AC58" s="1" t="s">
+      <c r="AC58" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="AD58" s="1" t="s">
+      <c r="AD58" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="AE58" s="1" t="s">
+      <c r="AE58" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="AF58" s="1" t="s">
+      <c r="AF58" s="6" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="59" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A59" s="1" t="s">
+    <row r="59" spans="1:32" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A59" s="6" t="s">
         <v>358</v>
       </c>
-      <c r="B59" s="1" t="s">
+      <c r="B59" s="6" t="s">
         <v>307</v>
       </c>
-      <c r="C59" s="2">
+      <c r="C59" s="7">
         <v>17</v>
       </c>
-      <c r="D59" s="2">
+      <c r="D59" s="7">
         <v>17</v>
       </c>
-      <c r="E59" s="1" t="s">
+      <c r="E59" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="F59" s="1" t="s">
+      <c r="F59" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="G59" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="H59" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="I59" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="J59" s="1" t="s">
+      <c r="G59" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="H59" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="I59" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="J59" s="6" t="s">
         <v>308</v>
       </c>
-      <c r="K59" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="L59" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="M59" s="1" t="s">
+      <c r="K59" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="L59" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="M59" s="6" t="s">
         <v>309</v>
       </c>
-      <c r="N59" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="O59" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="P59" s="1" t="s">
+      <c r="N59" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="O59" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="P59" s="6" t="s">
         <v>310</v>
       </c>
-      <c r="Q59" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="R59" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="S59" s="1" t="s">
+      <c r="Q59" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="R59" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="S59" s="6" t="s">
         <v>311</v>
       </c>
-      <c r="T59" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="U59" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="V59" s="1" t="s">
+      <c r="T59" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="U59" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="V59" s="6" t="s">
         <v>312</v>
       </c>
-      <c r="W59" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="X59" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="Y59" s="1" t="s">
+      <c r="W59" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="X59" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="Y59" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="Z59" s="1" t="s">
+      <c r="Z59" s="6" t="s">
         <v>117</v>
       </c>
-      <c r="AA59" s="1" t="s">
+      <c r="AA59" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="AB59" s="1" t="s">
+      <c r="AB59" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="AC59" s="1" t="s">
+      <c r="AC59" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="AD59" s="1" t="s">
+      <c r="AD59" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="AE59" s="1" t="s">
+      <c r="AE59" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="AF59" s="1" t="s">
+      <c r="AF59" s="6" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="60" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A60" s="1" t="s">
+    <row r="60" spans="1:32" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="6" t="s">
         <v>358</v>
       </c>
-      <c r="B60" s="1" t="s">
+      <c r="B60" s="6" t="s">
         <v>307</v>
       </c>
-      <c r="C60" s="2">
+      <c r="C60" s="7">
         <v>17</v>
       </c>
-      <c r="D60" s="2">
+      <c r="D60" s="7">
         <v>18</v>
       </c>
-      <c r="E60" s="1" t="s">
+      <c r="E60" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="F60" s="1" t="s">
+      <c r="F60" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="G60" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="H60" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="I60" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="J60" s="1" t="s">
+      <c r="G60" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="H60" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="I60" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="J60" s="6" t="s">
         <v>337</v>
       </c>
-      <c r="K60" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="L60" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="M60" s="1" t="s">
+      <c r="K60" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="L60" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="M60" s="6" t="s">
         <v>338</v>
       </c>
-      <c r="N60" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="O60" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="P60" s="1" t="s">
+      <c r="N60" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="O60" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="P60" s="6" t="s">
         <v>339</v>
       </c>
-      <c r="Q60" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="R60" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="S60" s="1" t="s">
+      <c r="Q60" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="R60" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="S60" s="6" t="s">
         <v>340</v>
       </c>
-      <c r="T60" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="U60" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="V60" s="1" t="s">
+      <c r="T60" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="U60" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="V60" s="6" t="s">
         <v>341</v>
       </c>
-      <c r="W60" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="X60" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="Y60" s="1" t="s">
+      <c r="W60" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="X60" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="Y60" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="Z60" s="1" t="s">
+      <c r="Z60" s="6" t="s">
         <v>117</v>
       </c>
-      <c r="AA60" s="1" t="s">
+      <c r="AA60" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="AB60" s="1" t="s">
+      <c r="AB60" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="AC60" s="1" t="s">
+      <c r="AC60" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="AD60" s="1" t="s">
+      <c r="AD60" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="AE60" s="1" t="s">
+      <c r="AE60" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="AF60" s="1" t="s">
+      <c r="AF60" s="6" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="61" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A61" s="1" t="s">
+    <row r="61" spans="1:32" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="6" t="s">
         <v>358</v>
       </c>
-      <c r="B61" s="1" t="s">
+      <c r="B61" s="6" t="s">
         <v>307</v>
       </c>
-      <c r="C61" s="2">
+      <c r="C61" s="7">
         <v>17</v>
       </c>
-      <c r="D61" s="2">
+      <c r="D61" s="7">
         <v>20</v>
       </c>
-      <c r="E61" s="1" t="s">
+      <c r="E61" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="F61" s="1" t="s">
+      <c r="F61" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="G61" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="H61" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="I61" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="J61" s="1" t="s">
+      <c r="G61" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="H61" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="I61" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="J61" s="6" t="s">
         <v>332</v>
       </c>
-      <c r="K61" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="L61" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="M61" s="1" t="s">
+      <c r="K61" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="L61" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="M61" s="6" t="s">
         <v>333</v>
       </c>
-      <c r="N61" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="O61" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="P61" s="1" t="s">
+      <c r="N61" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="O61" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="P61" s="6" t="s">
         <v>334</v>
       </c>
-      <c r="Q61" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="R61" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="S61" s="1" t="s">
+      <c r="Q61" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="R61" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="S61" s="6" t="s">
         <v>335</v>
       </c>
-      <c r="T61" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="U61" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="V61" s="1" t="s">
+      <c r="T61" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="U61" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="V61" s="6" t="s">
         <v>336</v>
       </c>
-      <c r="W61" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="X61" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="Y61" s="1" t="s">
+      <c r="W61" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="X61" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="Y61" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="Z61" s="1" t="s">
+      <c r="Z61" s="6" t="s">
         <v>117</v>
       </c>
-      <c r="AA61" s="1" t="s">
+      <c r="AA61" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="AB61" s="1" t="s">
+      <c r="AB61" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="AC61" s="1" t="s">
+      <c r="AC61" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="AD61" s="1" t="s">
+      <c r="AD61" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="AE61" s="1" t="s">
+      <c r="AE61" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="AF61" s="1" t="s">
+      <c r="AF61" s="6" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="62" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A62" s="1" t="s">
+    <row r="62" spans="1:32" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="6" t="s">
         <v>358</v>
       </c>
-      <c r="B62" s="1" t="s">
+      <c r="B62" s="6" t="s">
         <v>307</v>
       </c>
-      <c r="C62" s="2">
+      <c r="C62" s="7">
         <v>17</v>
       </c>
-      <c r="D62" s="2">
+      <c r="D62" s="7">
         <v>21</v>
       </c>
-      <c r="E62" s="1" t="s">
+      <c r="E62" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="F62" s="1" t="s">
+      <c r="F62" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="G62" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="H62" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="I62" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="J62" s="1" t="s">
+      <c r="G62" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="H62" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="I62" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="J62" s="6" t="s">
         <v>352</v>
       </c>
-      <c r="K62" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="L62" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="M62" s="1" t="s">
+      <c r="K62" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="L62" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="M62" s="6" t="s">
         <v>353</v>
       </c>
-      <c r="N62" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="O62" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="P62" s="1" t="s">
+      <c r="N62" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="O62" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="P62" s="6" t="s">
         <v>354</v>
       </c>
-      <c r="Q62" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="R62" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="S62" s="1" t="s">
+      <c r="Q62" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="R62" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="S62" s="6" t="s">
         <v>355</v>
       </c>
-      <c r="T62" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="U62" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="V62" s="1" t="s">
+      <c r="T62" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="U62" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="V62" s="6" t="s">
         <v>356</v>
       </c>
-      <c r="W62" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="X62" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="Y62" s="1" t="s">
+      <c r="W62" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="X62" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="Y62" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="Z62" s="1" t="s">
+      <c r="Z62" s="6" t="s">
         <v>117</v>
       </c>
-      <c r="AA62" s="1" t="s">
+      <c r="AA62" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="AB62" s="1" t="s">
+      <c r="AB62" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="AC62" s="1" t="s">
+      <c r="AC62" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="AD62" s="1" t="s">
+      <c r="AD62" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="AE62" s="1" t="s">
+      <c r="AE62" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="AF62" s="1" t="s">
+      <c r="AF62" s="6" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="63" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A63" s="1" t="s">
+    <row r="63" spans="1:32" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="6" t="s">
         <v>358</v>
       </c>
-      <c r="B63" s="1" t="s">
+      <c r="B63" s="6" t="s">
         <v>307</v>
       </c>
-      <c r="C63" s="2">
+      <c r="C63" s="7">
         <v>17</v>
       </c>
-      <c r="D63" s="2">
+      <c r="D63" s="7">
         <v>27</v>
       </c>
-      <c r="E63" s="1" t="s">
+      <c r="E63" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="F63" s="1" t="s">
+      <c r="F63" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="G63" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="H63" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="I63" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="J63" s="1" t="s">
+      <c r="G63" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="H63" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="I63" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="J63" s="6" t="s">
         <v>318</v>
       </c>
-      <c r="K63" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="L63" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="M63" s="1" t="s">
+      <c r="K63" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="L63" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="M63" s="6" t="s">
         <v>319</v>
       </c>
-      <c r="N63" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="O63" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="P63" s="1" t="s">
+      <c r="N63" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="O63" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="P63" s="6" t="s">
         <v>320</v>
       </c>
-      <c r="Q63" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="R63" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="S63" s="1" t="s">
+      <c r="Q63" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="R63" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="S63" s="6" t="s">
         <v>321</v>
       </c>
-      <c r="T63" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="U63" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="V63" s="1" t="s">
+      <c r="T63" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="U63" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="V63" s="6" t="s">
         <v>322</v>
       </c>
-      <c r="W63" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="X63" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="Y63" s="1" t="s">
+      <c r="W63" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="X63" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="Y63" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="Z63" s="1" t="s">
+      <c r="Z63" s="6" t="s">
         <v>117</v>
       </c>
-      <c r="AA63" s="1" t="s">
+      <c r="AA63" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="AB63" s="1" t="s">
+      <c r="AB63" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="AC63" s="1" t="s">
+      <c r="AC63" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="AD63" s="1" t="s">
+      <c r="AD63" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="AE63" s="1" t="s">
+      <c r="AE63" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="AF63" s="1" t="s">
+      <c r="AF63" s="6" t="s">
         <v>47</v>
       </c>
     </row>

</xml_diff>